<commit_message>
IMPLEMENTACION DE HISTORIAL DE ENTRADAS Y SALIDAS DEL SISTEMA
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/USUARIOS.xlsx
+++ b/ProyectoPooDist/excels/USUARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B0B924-ED3C-4C71-B751-623562232843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE3A70D-B28F-4714-8C9F-CC6A88C6CA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Nombre de Usuario</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Daniel</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>EN VACACIONES</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Teresa</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>BLOQUEADO</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Antonio</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Isabel</t>
   </si>
   <si>
@@ -136,9 +124,6 @@
     <t>isabel.ortega@gmail.com</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Roberto</t>
   </si>
   <si>
@@ -155,16 +140,52 @@
   </si>
   <si>
     <t>ENFERMO</t>
+  </si>
+  <si>
+    <t>csgoisgoodgames123</t>
+  </si>
+  <si>
+    <t>csgoisgoodgames124</t>
+  </si>
+  <si>
+    <t>csgoisgoodgames125</t>
+  </si>
+  <si>
+    <t>csgoisgoodgames126</t>
+  </si>
+  <si>
+    <t>csgoisgoodgames127</t>
+  </si>
+  <si>
+    <t>josegonzalezcoradopineed</t>
+  </si>
+  <si>
+    <t>javiergonzalezcoradopineed</t>
+  </si>
+  <si>
+    <t>davidgonzalezcoradopineed</t>
+  </si>
+  <si>
+    <t>luisagonzalezcoradopineed</t>
+  </si>
+  <si>
+    <t>silviagonzalezcoradopineed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -529,7 +550,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,180 +592,181 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
       </c>
       <c r="G2">
         <v>4444444444444</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2">
         <v>67367363</v>
       </c>
       <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
       </c>
       <c r="G3">
         <v>5555555555555</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I3">
         <v>67373673</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
       </c>
       <c r="G4">
         <v>6666666666666</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I4">
         <v>32521321</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>7777777777777</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I5">
         <v>53423423</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>8888888888888</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I6">
         <v>21321321</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑO NO.3
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/USUARIOS.xlsx
+++ b/ProyectoPooDist/excels/USUARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AA4396-0C2A-4B67-BD53-399CA5BF27CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3C4FCA-DB9F-420D-A02A-A2C519661718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Nombre de Usuario</t>
   </si>
@@ -55,106 +55,82 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Ruiz</t>
-  </si>
-  <si>
-    <t>USUARIO</t>
+    <t>saragonzalezcoradopineed</t>
+  </si>
+  <si>
+    <t>1234##AApineed</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Castro</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
   </si>
   <si>
     <t>Masculino</t>
   </si>
   <si>
-    <t>11/11/2000</t>
-  </si>
-  <si>
-    <t>daniel.ruiz@gmail.com</t>
-  </si>
-  <si>
-    <t>EN VACACIONES</t>
+    <t>13/01/2002</t>
+  </si>
+  <si>
+    <t>antonio.castro@gmail.com</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>davidganzalezcoradopineed</t>
+  </si>
+  <si>
+    <t>1000##AApineed</t>
+  </si>
+  <si>
+    <t>Isabel</t>
+  </si>
+  <si>
+    <t>Ortega</t>
+  </si>
+  <si>
+    <t>SECRETARIA</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>14/02/2003</t>
+  </si>
+  <si>
+    <t>isabel.ortega@gmail.com</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Teresa</t>
-  </si>
-  <si>
-    <t>Morales</t>
-  </si>
-  <si>
-    <t>ADMINISTRADOR</t>
-  </si>
-  <si>
-    <t>Femenino</t>
-  </si>
-  <si>
-    <t>12/12/2001</t>
-  </si>
-  <si>
-    <t>teresa.morales@gmail.com</t>
-  </si>
-  <si>
-    <t>ACTIVO</t>
-  </si>
-  <si>
-    <t>davidgonzalezcoradopineed</t>
-  </si>
-  <si>
-    <t>csgoisgoodgames125</t>
-  </si>
-  <si>
-    <t>Antonio</t>
-  </si>
-  <si>
-    <t>Castro</t>
-  </si>
-  <si>
-    <t>13/01/2002</t>
-  </si>
-  <si>
-    <t>antonio.castro@gmail.com</t>
-  </si>
-  <si>
-    <t>BLOQUEADO</t>
-  </si>
-  <si>
-    <t>luisagonzalezcoradopineed</t>
-  </si>
-  <si>
-    <t>12312##AApineed</t>
-  </si>
-  <si>
-    <t>Isabel</t>
-  </si>
-  <si>
-    <t>Ortega</t>
-  </si>
-  <si>
-    <t>14/02/2003</t>
-  </si>
-  <si>
-    <t>isabel.ortega@gmail.com</t>
-  </si>
-  <si>
-    <t>Roberto</t>
-  </si>
-  <si>
-    <t>Sánchez</t>
-  </si>
-  <si>
-    <t>SECRETARIA</t>
-  </si>
-  <si>
-    <t>15/03/2004</t>
-  </si>
-  <si>
-    <t>roberto.sanchez@gmail.com</t>
-  </si>
-  <si>
-    <t>ENFERMO</t>
+    <t>Meme</t>
+  </si>
+  <si>
+    <t>González</t>
+  </si>
+  <si>
+    <t>meme.gonzalez@gmail.com</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Corado</t>
+  </si>
+  <si>
+    <t>david.corado@gmail.com</t>
+  </si>
+  <si>
+    <t>memeganzalezcoradopineed</t>
   </si>
 </sst>
 </file>
@@ -526,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,99 +546,99 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2">
-        <v>4444444444444</v>
+        <v>8498489595912</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2">
-        <v>67367363</v>
+        <v>32521321</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>4898949848942</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3">
+        <v>53423423</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3">
-        <v>5555555555555</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3">
-        <v>67373673</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>6666666666666</v>
+        <v>1515565648484</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>32521321</v>
@@ -671,77 +647,42 @@
         <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5">
-        <v>7777777777777</v>
+        <v>1981989848591</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I5">
         <v>53423423</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>8888888888888</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6">
-        <v>21321321</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑO NO.4
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/USUARIOS.xlsx
+++ b/ProyectoPooDist/excels/USUARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3C4FCA-DB9F-420D-A02A-A2C519661718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB8135F-CAB7-404B-A78F-DA59E46BFDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Nombre de Usuario</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>david.corado@gmail.com</t>
-  </si>
-  <si>
-    <t>memeganzalezcoradopineed</t>
   </si>
 </sst>
 </file>
@@ -505,7 +502,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,8 +613,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -651,8 +648,8 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
+      <c r="A5">
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
OPTIMIZACION DE PROCESOS Y DISEÑO NO.10
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/USUARIOS.xlsx
+++ b/ProyectoPooDist/excels/USUARIOS.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C6C211-27DA-4DFD-8E00-8D059B8E0250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2EFC3-41FE-49CD-9074-6A6775A0C6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Nombre de Usuario</t>
   </si>
@@ -128,12 +128,28 @@
   </si>
   <si>
     <t>carolina.castro&amp;pineed</t>
+  </si>
+  <si>
+    <t>ENFERMO</t>
+  </si>
+  <si>
+    <t>EN VACACIONES</t>
+  </si>
+  <si>
+    <t>JUBILADO</t>
+  </si>
+  <si>
+    <t>BLOQUEADO</t>
+  </si>
+  <si>
+    <t>INACTIVO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,58 +524,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>8012345678900</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -579,7 +596,7 @@
       <c r="H2" s="3">
         <v>31168</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>33664538</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -588,8 +605,11 @@
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="L2" t="b" s="0">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -614,17 +634,20 @@
       <c r="H3" s="3">
         <v>32942</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>20115747</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+      <c r="L3" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -649,17 +672,20 @@
       <c r="H4" s="3">
         <v>31943</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>74767823</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
+      </c>
+      <c r="L4" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -684,17 +710,17 @@
       <c r="H5" s="3">
         <v>32538</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>78610529</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -719,13 +745,51 @@
       <c r="H6" s="3">
         <v>30205</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>32798897</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8012345678900</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8123450000000</v>
+      </c>
+      <c r="H7" s="3">
+        <v>31168</v>
+      </c>
+      <c r="I7" s="0">
+        <v>33664538</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SOLUCION DE CONFLICTOS EXCEL Y GESTION USUARIOS INICIO/INACTIVOS PILTOSINACTIVOS
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/USUARIOS.xlsx
+++ b/ProyectoPooDist/excels/USUARIOS.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2EFC3-41FE-49CD-9074-6A6775A0C6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4354D35D-2B09-4CB8-A259-4ADED298DA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Nombre de Usuario</t>
   </si>
@@ -139,17 +139,22 @@
     <t>JUBILADO</t>
   </si>
   <si>
-    <t>BLOQUEADO</t>
-  </si>
-  <si>
-    <t>INACTIVO</t>
+    <t>jose.gonzalez&amp;pineed</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>González</t>
+  </si>
+  <si>
+    <t>jose.gonzalez@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,54 +529,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.5703125"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -579,10 +584,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -591,21 +596,21 @@
         <v>13</v>
       </c>
       <c r="G2" s="2">
-        <v>8123450000000</v>
+        <v>3256451010312</v>
       </c>
       <c r="H2" s="3">
         <v>31168</v>
       </c>
-      <c r="I2" s="0">
-        <v>33664538</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
+      <c r="I2">
+        <v>59596565</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="b" s="0">
+      <c r="L2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -634,7 +639,7 @@
       <c r="H3" s="3">
         <v>32942</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>20115747</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -643,7 +648,7 @@
       <c r="K3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L3" t="b" s="0">
+      <c r="L3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -672,7 +677,7 @@
       <c r="H4" s="3">
         <v>31943</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>74767823</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -681,7 +686,7 @@
       <c r="K4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L4" t="b" s="0">
+      <c r="L4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -710,7 +715,7 @@
       <c r="H5" s="3">
         <v>32538</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>78610529</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -718,6 +723,9 @@
       </c>
       <c r="K5" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -745,7 +753,7 @@
       <c r="H6" s="3">
         <v>30205</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>32798897</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -754,7 +762,7 @@
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L6" t="b" s="0">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -783,7 +791,7 @@
       <c r="H7" s="3">
         <v>31168</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>33664538</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -791,6 +799,47 @@
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3256451010312</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3256451010312</v>
+      </c>
+      <c r="H8" s="3">
+        <v>31168</v>
+      </c>
+      <c r="I8">
+        <v>59596565</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>